<commit_message>
Remove ministry revenue - it's part of other revenue (no separate breakdown)
</commit_message>
<xml_diff>
--- a/data/processed/1404-table5.xlsx
+++ b/data/processed/1404-table5.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hamidreza/Documents/AI-Projects/IranBudget/data/processed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA27E01-132B-6A4D-A1E5-184FCE2A555E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50C001B9-9907-044A-A2F2-5A70BA189FA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8480" yWindow="900" windowWidth="42560" windowHeight="20080" xr2:uid="{A1C43625-39F6-5F48-97AB-0D07967D3E07}"/>
+    <workbookView xWindow="19460" yWindow="500" windowWidth="23740" windowHeight="20080" activeTab="3" xr2:uid="{A1C43625-39F6-5F48-97AB-0D07967D3E07}"/>
   </bookViews>
   <sheets>
     <sheet name="1404" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="1403" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet1 (2)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="233">
   <si>
     <t>قسمت اول: درآمد‌ها</t>
   </si>
@@ -492,6 +494,249 @@
   </si>
   <si>
     <t>جمع کل</t>
+  </si>
+  <si>
+    <t>جمع</t>
+  </si>
+  <si>
+    <t>نهاد ریاست جمهوری</t>
+  </si>
+  <si>
+    <t>شورای مالی امنیت ملی</t>
+  </si>
+  <si>
+    <t>دبیرخانه مجلس خبرگان</t>
+  </si>
+  <si>
+    <t>مجمع تشخیص مصلحت</t>
+  </si>
+  <si>
+    <t>بنیاد ملی نخبگان</t>
+  </si>
+  <si>
+    <t>معاونت علمی و فناوری رییس جمهور</t>
+  </si>
+  <si>
+    <t>سازمان اداری و استخدامی کشور</t>
+  </si>
+  <si>
+    <t>مرکز ملی فضای مجازی کشور</t>
+  </si>
+  <si>
+    <t>مجلس شورای اسلامی</t>
+  </si>
+  <si>
+    <t>دیوان محاسبات کشور</t>
+  </si>
+  <si>
+    <t>شورای نگهبان</t>
+  </si>
+  <si>
+    <t>وزارت اطلاعات</t>
+  </si>
+  <si>
+    <t>سازمان برنامه و بودجه کشور</t>
+  </si>
+  <si>
+    <t>وزارت کشور</t>
+  </si>
+  <si>
+    <t>فرماندهی کل انتظامی جمهوری اسلامی ایران</t>
+  </si>
+  <si>
+    <t>وزارت امور خارجه</t>
+  </si>
+  <si>
+    <t>وزارت دادگستری</t>
+  </si>
+  <si>
+    <t>دادگستری جمهوری اسلامی ایران</t>
+  </si>
+  <si>
+    <t>دیوان عدالت اداری</t>
+  </si>
+  <si>
+    <t>سازمان بازرسی کل کشور</t>
+  </si>
+  <si>
+    <t>سازمان اوقاف و امور خیریه</t>
+  </si>
+  <si>
+    <t>وزارت امور اقتصادی و دارایی</t>
+  </si>
+  <si>
+    <t>وزارت دفاع و پشتیبانی نیروهای مسلح</t>
+  </si>
+  <si>
+    <t>ستاد مشترک ارتش جمهوری اسلامی ایران</t>
+  </si>
+  <si>
+    <t>ستاد مشترک سپاه پاسداران انتقلاب اسلامی</t>
+  </si>
+  <si>
+    <t>ستاد فرماندهی کل نیروهای مسلح جمهوری اسلامی</t>
+  </si>
+  <si>
+    <t>بنیاد حفظ آثار و ارزش‌های دفاع مقدس</t>
+  </si>
+  <si>
+    <t>قرارگاه مرکزی حضرت خاتم‌النبیا</t>
+  </si>
+  <si>
+    <t>قرب بقیه‌الله - کمک و حمایت از موسسات فرهنگی و اجتماعی</t>
+  </si>
+  <si>
+    <t>وزارت علوم تحقیقات و فناوری</t>
+  </si>
+  <si>
+    <t>دبیرخانه شروارای عالی انقلاب فرهنگی</t>
+  </si>
+  <si>
+    <t>جهاد دانشگاهی</t>
+  </si>
+  <si>
+    <t>وزارت میراث فرهنگی گردشگری و صنایع‌دستی</t>
+  </si>
+  <si>
+    <t>وزارت فرهنگ و ارشاد اسلامی</t>
+  </si>
+  <si>
+    <t>دفتر تبلیغات اسلامی حوزه علمیه قم</t>
+  </si>
+  <si>
+    <t>شورای هماهنگی تبلیغات اسلامی</t>
+  </si>
+  <si>
+    <t>شورای عالی حوزه‌های علمیه</t>
+  </si>
+  <si>
+    <t>شورای عالی حوزه علمیه خراسان</t>
+  </si>
+  <si>
+    <t>مرکز خدمات حوزه‌های علمیه</t>
+  </si>
+  <si>
+    <t>موسسه آموزشی و پژوهشی امام خمینی</t>
+  </si>
+  <si>
+    <t>سازمان تبلیغات اسلامی</t>
+  </si>
+  <si>
+    <t>جامعه المصطفی العالمیه</t>
+  </si>
+  <si>
+    <t>وزارت آموزش و پرورش</t>
+  </si>
+  <si>
+    <t>وزارت ورزش و جوانان</t>
+  </si>
+  <si>
+    <t>وزارت بهداشت و درمان و آموزش پزشکی</t>
+  </si>
+  <si>
+    <t>کمیته امداد امام خمینی</t>
+  </si>
+  <si>
+    <t>جمعیت هلال احمر جمهوری اسلامی ایران</t>
+  </si>
+  <si>
+    <t>سازمان بهزیستی کشور</t>
+  </si>
+  <si>
+    <t>بنیاد شهید و امور ایثارگران</t>
+  </si>
+  <si>
+    <t>بنیاد مسکن اسلامی</t>
+  </si>
+  <si>
+    <t>سازمان حفاظت محیط زیست</t>
+  </si>
+  <si>
+    <t>وزارت نفت</t>
+  </si>
+  <si>
+    <t>وزارت نیرو</t>
+  </si>
+  <si>
+    <t>سازمان انرژی اتمی ایران</t>
+  </si>
+  <si>
+    <t>سازمان ملی استاندارد</t>
+  </si>
+  <si>
+    <t>وزارت ارتباطات و فاناوری اطلاعات</t>
+  </si>
+  <si>
+    <t>وزارت جهاد کشاورزی</t>
+  </si>
+  <si>
+    <t>وزارت راه و شهرسازی</t>
+  </si>
+  <si>
+    <t>وزارت تعاون کار و رفاه اجتماعی</t>
+  </si>
+  <si>
+    <t>وزارت صنعت معدن و تجارت</t>
+  </si>
+  <si>
+    <t>سازمان صدا و سیمای جمهوری اسلامی ایران</t>
+  </si>
+  <si>
+    <t>اعتبارات متفرقه</t>
+  </si>
+  <si>
+    <t>امنیت</t>
+  </si>
+  <si>
+    <t>آموزش</t>
+  </si>
+  <si>
+    <t>ارشاد</t>
+  </si>
+  <si>
+    <t>مالیات اشخاص حقوقی</t>
+  </si>
+  <si>
+    <t>مالیات بر درآمدها</t>
+  </si>
+  <si>
+    <t>مالیات بر ثروت</t>
+  </si>
+  <si>
+    <t>مالیات بر واردات</t>
+  </si>
+  <si>
+    <t>مالیات بر کالاها و خدمات</t>
+  </si>
+  <si>
+    <t>درآمد های ناشی از کمکهای اجتماعی</t>
+  </si>
+  <si>
+    <t>درآمدهای حاصل از مالکیت دولت</t>
+  </si>
+  <si>
+    <t>درآمدهای حاصل از فروش کالاها و خدمات</t>
+  </si>
+  <si>
+    <t>درآمدهای حاصل از جرایم و خسارات</t>
+  </si>
+  <si>
+    <t>درآمدهای متفرقه</t>
+  </si>
+  <si>
+    <t>منابع حاصل از نفت و فرآورده‌های نفتی</t>
+  </si>
+  <si>
+    <t>منابع حاصل از فروش و واگذاری اموال منقول و غیر منقول</t>
+  </si>
+  <si>
+    <t>منابع حاصل از واگذاری طرح‌های تملک دارایی‌های سرمایه‌ای</t>
+  </si>
+  <si>
+    <t>واگذاری دارایی‌های مالی</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -502,7 +747,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -521,6 +766,14 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="IRANSans"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -550,11 +803,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -870,14 +1124,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0553A598-02EF-434F-8A8F-78C667E432DD}">
-  <dimension ref="A2:F170"/>
+  <dimension ref="A2:F238"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A155" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A174" sqref="A174"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A169" sqref="A169:B169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="23.33203125" customWidth="1"/>
     <col min="2" max="2" width="28.1640625" style="2" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.83203125" customWidth="1"/>
@@ -2510,7 +2765,7 @@
         <v>1499000</v>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>310520</v>
       </c>
@@ -2521,7 +2776,7 @@
         <v>800000000</v>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>310521</v>
       </c>
@@ -2532,7 +2787,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>310600</v>
       </c>
@@ -2543,7 +2798,7 @@
         <v>131500000</v>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>319601</v>
       </c>
@@ -2554,7 +2809,7 @@
         <v>25000000</v>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>319602</v>
       </c>
@@ -2565,7 +2820,7 @@
         <v>31500000</v>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>310605</v>
       </c>
@@ -2576,7 +2831,7 @@
         <v>44000000</v>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>310606</v>
       </c>
@@ -2587,7 +2842,7 @@
         <v>31000000</v>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>310700</v>
       </c>
@@ -2598,7 +2853,7 @@
         <v>5410000000</v>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>310705</v>
       </c>
@@ -2609,12 +2864,552 @@
         <v>5410000000</v>
       </c>
     </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B170" s="2" t="s">
         <v>151</v>
       </c>
       <c r="C170" s="1">
         <v>53834550000</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" ht="16" x14ac:dyDescent="0.2">
+      <c r="B174"/>
+      <c r="C174"/>
+    </row>
+    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B175" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="C175" s="1">
+        <v>85591174</v>
+      </c>
+      <c r="D175" s="4"/>
+      <c r="E175" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B176" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C176" s="1">
+        <v>2304855</v>
+      </c>
+      <c r="D176" s="1"/>
+      <c r="E176" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="177" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B177" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="C177" s="1">
+        <v>449509</v>
+      </c>
+      <c r="D177" s="1"/>
+      <c r="E177" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="178" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B178" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C178" s="1">
+        <v>10934996</v>
+      </c>
+      <c r="D178" s="1"/>
+      <c r="E178" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="179" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B179" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C179" s="1">
+        <v>6761890</v>
+      </c>
+      <c r="D179" s="1"/>
+    </row>
+    <row r="180" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B180" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C180" s="1">
+        <v>44948334</v>
+      </c>
+      <c r="D180" s="1"/>
+    </row>
+    <row r="181" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B181" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C181" s="1">
+        <v>7447890</v>
+      </c>
+      <c r="D181" s="1"/>
+    </row>
+    <row r="182" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B182" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C182" s="1">
+        <v>6963000</v>
+      </c>
+      <c r="D182" s="1"/>
+    </row>
+    <row r="183" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B183" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="C183" s="1">
+        <v>70126639</v>
+      </c>
+      <c r="D183" s="1"/>
+    </row>
+    <row r="184" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B184" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C184" s="1">
+        <v>50906000</v>
+      </c>
+      <c r="D184" s="1"/>
+    </row>
+    <row r="185" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B185" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C185" s="1">
+        <v>9225689</v>
+      </c>
+      <c r="D185" s="1"/>
+    </row>
+    <row r="186" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B186" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C186" s="1">
+        <v>542587249</v>
+      </c>
+      <c r="D186" s="1"/>
+    </row>
+    <row r="187" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B187" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="C187" s="1">
+        <v>257815119</v>
+      </c>
+      <c r="D187" s="1"/>
+    </row>
+    <row r="188" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B188" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="C188" s="1">
+        <v>344222514</v>
+      </c>
+      <c r="D188" s="1"/>
+    </row>
+    <row r="189" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B189" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="C189" s="1">
+        <v>1155214629</v>
+      </c>
+      <c r="D189" s="1"/>
+    </row>
+    <row r="190" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B190" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="C190" s="1">
+        <v>60142091</v>
+      </c>
+    </row>
+    <row r="191" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B191" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C191" s="1">
+        <v>48643608</v>
+      </c>
+      <c r="D191" s="4"/>
+    </row>
+    <row r="192" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B192" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C192" s="1">
+        <v>1201572871</v>
+      </c>
+      <c r="D192" s="4"/>
+    </row>
+    <row r="193" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B193" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C193" s="1">
+        <v>11666330</v>
+      </c>
+      <c r="D193" s="4"/>
+    </row>
+    <row r="194" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B194" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="C194" s="1">
+        <v>51996500</v>
+      </c>
+      <c r="D194" s="4"/>
+    </row>
+    <row r="195" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B195" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C195" s="1">
+        <v>1158500</v>
+      </c>
+      <c r="D195" s="4"/>
+    </row>
+    <row r="196" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B196" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="C196" s="1">
+        <v>739964601</v>
+      </c>
+    </row>
+    <row r="197" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B197" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C197" s="1">
+        <v>2452268893</v>
+      </c>
+    </row>
+    <row r="198" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B198" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="C198" s="1">
+        <v>800518757</v>
+      </c>
+    </row>
+    <row r="199" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B199" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="C199" s="1">
+        <v>1985985754</v>
+      </c>
+    </row>
+    <row r="200" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B200" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C200" s="1">
+        <v>34195599</v>
+      </c>
+    </row>
+    <row r="201" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B201" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C201" s="1">
+        <v>9125000</v>
+      </c>
+    </row>
+    <row r="202" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B202" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="C202" s="1">
+        <v>16934901</v>
+      </c>
+    </row>
+    <row r="203" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B203" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C203" s="1">
+        <v>19542589</v>
+      </c>
+    </row>
+    <row r="204" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B204" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C204" s="1">
+        <v>1192847837</v>
+      </c>
+    </row>
+    <row r="205" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B205" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C205" s="1">
+        <v>10433062</v>
+      </c>
+    </row>
+    <row r="206" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B206" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="C206" s="1">
+        <v>28659041</v>
+      </c>
+    </row>
+    <row r="207" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B207" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="C207" s="1">
+        <v>79477500</v>
+      </c>
+    </row>
+    <row r="208" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B208" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="C208" s="1">
+        <v>141324483</v>
+      </c>
+    </row>
+    <row r="209" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B209" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C209" s="1">
+        <v>9141000</v>
+      </c>
+    </row>
+    <row r="210" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B210" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="C210" s="1">
+        <v>3320000</v>
+      </c>
+    </row>
+    <row r="211" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B211" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="C211" s="1">
+        <v>88616000</v>
+      </c>
+    </row>
+    <row r="212" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B212" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="C212" s="1">
+        <v>8873000</v>
+      </c>
+    </row>
+    <row r="213" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B213" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C213" s="1">
+        <v>140973158</v>
+      </c>
+    </row>
+    <row r="214" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B214" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C214" s="1">
+        <v>4041095</v>
+      </c>
+    </row>
+    <row r="215" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B215" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C215" s="1">
+        <v>62580596</v>
+      </c>
+    </row>
+    <row r="216" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B216" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C216" s="1">
+        <v>17555000</v>
+      </c>
+    </row>
+    <row r="217" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B217" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C217" s="1">
+        <v>3941864917</v>
+      </c>
+    </row>
+    <row r="218" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B218" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C218" s="1">
+        <v>224275600</v>
+      </c>
+    </row>
+    <row r="219" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B219" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C219" s="1">
+        <v>5791382271</v>
+      </c>
+    </row>
+    <row r="220" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B220" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C220" s="1">
+        <v>240308607</v>
+      </c>
+    </row>
+    <row r="221" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B221" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="C221" s="1">
+        <v>176777315</v>
+      </c>
+    </row>
+    <row r="222" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B222" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="C222" s="1">
+        <v>435908427</v>
+      </c>
+    </row>
+    <row r="223" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B223" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C223" s="1">
+        <v>1243200000</v>
+      </c>
+    </row>
+    <row r="224" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B224" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C224" s="1">
+        <v>31770100</v>
+      </c>
+    </row>
+    <row r="225" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B225" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="C225" s="1">
+        <v>81985185</v>
+      </c>
+    </row>
+    <row r="226" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B226" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="C226" s="1">
+        <v>5719000</v>
+      </c>
+    </row>
+    <row r="227" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B227" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C227" s="1">
+        <v>838511022</v>
+      </c>
+    </row>
+    <row r="228" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B228" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C228" s="1">
+        <v>35397716</v>
+      </c>
+    </row>
+    <row r="229" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B229" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C229" s="1">
+        <v>33233362</v>
+      </c>
+    </row>
+    <row r="230" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B230" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="C230" s="1">
+        <v>237676720</v>
+      </c>
+    </row>
+    <row r="231" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B231" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C231" s="1">
+        <v>365832094</v>
+      </c>
+    </row>
+    <row r="232" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B232" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="C232" s="1">
+        <v>980086734</v>
+      </c>
+    </row>
+    <row r="233" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B233" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C233" s="1">
+        <v>4519201906</v>
+      </c>
+    </row>
+    <row r="234" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B234" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C234" s="1">
+        <v>224425269</v>
+      </c>
+    </row>
+    <row r="235" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B235" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C235" s="1">
+        <v>296317000</v>
+      </c>
+    </row>
+    <row r="236" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B236" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C236" s="1">
+        <v>31441356998</v>
+      </c>
+    </row>
+    <row r="238" spans="2:3" x14ac:dyDescent="0.35">
+      <c r="B238" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="C238" s="1">
+        <v>2691459620</v>
       </c>
     </row>
   </sheetData>
@@ -2626,8 +3421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A9B7C99-11C9-D04A-8A37-264C545D621A}">
   <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2885,82 +3680,830 @@
     </row>
     <row r="34" spans="1:3" ht="19" x14ac:dyDescent="0.35">
       <c r="B34" s="2" t="s">
-        <v>2</v>
+        <v>218</v>
       </c>
       <c r="C34" s="3">
         <v>8166508049</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="B35" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C35" s="3">
+        <v>3223566661</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="B36" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C36" s="3">
+        <v>551716162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="B37" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2719050000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="B38" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="C38" s="3">
+        <v>6466124306</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="B39" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C39" s="3">
+        <v>117840000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="B40" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1951827876</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="B41" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="C41" s="3">
+        <v>3142025220</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="B42" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="C42" s="3">
+        <v>359342000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="B43" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="C43" s="3">
+        <v>2041219726</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A44" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="B45" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C45" s="3">
+        <v>6045000000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="B46" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="C46" s="3">
+        <v>3254582000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="B47" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="C47" s="3">
+        <v>5498000</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A48" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="B49" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C49" s="3">
+        <v>15800250000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{113B239A-9FB9-D54C-BF02-DED76B2A408E}">
+  <dimension ref="A1:C31"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="39.1640625" customWidth="1"/>
+    <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>100000</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1">
+        <v>18729709000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>110000</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>13836326031</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>110100</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>4723804498</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>110200</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1916253759</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>110300</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1">
+        <v>404748310</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>110400</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1470649449</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>110500</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5320870015</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>120000</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="1">
+        <v>80000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>130000</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1749747688</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>130100</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="1">
+        <v>600000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>130300</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="1">
+        <v>14975618</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>130400</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1134772070</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>140000</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="1">
+        <v>1966531398</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>140100</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1929852208</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>140200</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C15" s="1">
+        <v>36679190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>150000</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="1">
+        <v>266672409</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>160000</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="1">
+        <v>830431474</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>200000</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="1">
+        <v>6449721000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>210000</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="1">
+        <v>6449721000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>210100</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C20" s="1">
+        <v>5827430000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>210200</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="1">
+        <v>622290000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>210300</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>300000</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3191970000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>310000</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="1">
+        <v>3191970000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>310100</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2546002000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>310200</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>310400</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C27" s="1">
+        <v>14963000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>310500</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" s="1">
+        <v>600000000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>310600</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="C29" s="1">
+        <v>31004000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>310700</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>310705</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE8BE4D5-BEFD-CF4F-8E81-C6FDA005DE2C}">
+  <dimension ref="A1:D49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C45" sqref="B45:C47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="40.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3">
+        <v>28739220000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>21126965178</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="C3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3">
+        <v>8166508049</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="C4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3223566661</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="3">
+        <v>551716162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="C6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2719050000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="C7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="3">
+        <v>6466124306</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="B8" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="3">
+        <v>117840000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="B9" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1951827876</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="C10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" s="3">
+        <v>999999000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="C11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="3">
+        <v>32111589</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="C12" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="3">
+        <v>919717287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="B13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C13" s="3">
+        <v>3142025220</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="C14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="3">
+        <v>3080141035</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="C15" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15" s="3">
+        <v>61884185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="B16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" s="3">
+        <v>359342000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="B17" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" s="3">
+        <v>2041219726</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B18" s="3">
+        <v>9305080000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="B19" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="3">
+        <v>9305080000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="C20" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="3">
+        <v>6045000000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="C21" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="3">
+        <v>3254582000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="C22" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D22" s="3">
+        <v>5498000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23" s="3">
+        <v>15800250000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="B24" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="C24" s="3">
+        <v>15800250000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="C25" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" s="3">
+        <v>8100003000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="C26" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D26" s="3">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="C27" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D27" s="3">
+        <v>7237000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="C28" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D28" s="3">
+        <v>2151500000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="C29" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D29" s="3">
+        <v>131500000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="19" x14ac:dyDescent="0.35">
+      <c r="C30" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D30" s="3">
+        <v>5410000000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="A33" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="19" x14ac:dyDescent="0.35">
+      <c r="B34" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" s="1">
+        <v>4723804498</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="19" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C35" s="3">
-        <v>3223566661</v>
+      <c r="C35" s="1">
+        <v>1916253759</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="19" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C36" s="3">
-        <v>551716162</v>
+      <c r="C36" s="1">
+        <v>404748310</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="19" x14ac:dyDescent="0.35">
       <c r="B37" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C37" s="3">
-        <v>2719050000</v>
+      <c r="C37" s="1">
+        <v>1470649449</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="19" x14ac:dyDescent="0.35">
       <c r="B38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C38" s="3">
-        <v>6466124306</v>
+      <c r="C38" s="1">
+        <v>5320870015</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="19" x14ac:dyDescent="0.35">
       <c r="B39" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="3">
-        <v>117840000</v>
+      <c r="C39" s="1">
+        <v>80000000</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="19" x14ac:dyDescent="0.35">
       <c r="B40" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="3">
-        <v>1951827876</v>
+      <c r="C40" s="1">
+        <v>1749747688</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="19" x14ac:dyDescent="0.35">
       <c r="B41" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C41" s="3">
-        <v>3142025220</v>
+      <c r="C41" s="1">
+        <v>1966531398</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="19" x14ac:dyDescent="0.35">
       <c r="B42" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C42" s="3">
-        <v>359342000</v>
+      <c r="C42" s="1">
+        <v>266672409</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="19" x14ac:dyDescent="0.35">
       <c r="B43" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C43" s="3">
-        <v>2041219726</v>
+      <c r="C43" s="1">
+        <v>830431474</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="19" x14ac:dyDescent="0.35">
@@ -2972,24 +4515,24 @@
       <c r="B45" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C45" s="3">
-        <v>6045000000</v>
+      <c r="C45" s="1">
+        <v>5827430000</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="19" x14ac:dyDescent="0.35">
       <c r="B46" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C46" s="3">
-        <v>3254582000</v>
+      <c r="C46" s="1">
+        <v>622290000</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="19" x14ac:dyDescent="0.35">
       <c r="B47" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C47" s="3">
-        <v>5498000</v>
+      <c r="C47" s="1">
+        <v>1000</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="19" x14ac:dyDescent="0.35">
@@ -2999,7 +4542,7 @@
     </row>
     <row r="49" spans="2:3" ht="19" x14ac:dyDescent="0.35">
       <c r="B49" s="2" t="s">
-        <v>126</v>
+        <v>231</v>
       </c>
       <c r="C49" s="3">
         <v>15800250000</v>

</xml_diff>